<commit_message>
Add intial patch for fixtures
</commit_message>
<xml_diff>
--- a/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.10.xlsx
+++ b/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="101">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -37,9 +37,24 @@
     <t xml:space="preserve">Rigging Points</t>
   </si>
   <si>
+    <t xml:space="preserve">Channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Power</t>
+  </si>
+  <si>
     <t xml:space="preserve">Upstage Structure</t>
   </si>
   <si>
+    <t xml:space="preserve">6 Universes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elation Sniper 2R</t>
   </si>
   <si>
@@ -106,12 +121,15 @@
     <t xml:space="preserve">Shackle 5/8"</t>
   </si>
   <si>
+    <t xml:space="preserve">ADJ 5P Hex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backstage &amp; Stair </t>
+  </si>
+  <si>
     <t xml:space="preserve">Work Lights</t>
   </si>
   <si>
-    <t xml:space="preserve">Backstage &amp; Stair </t>
-  </si>
-  <si>
     <t xml:space="preserve">Christie B Truss 8'</t>
   </si>
   <si>
@@ -130,9 +148,15 @@
     <t xml:space="preserve">Motor 1 Ton</t>
   </si>
   <si>
+    <t xml:space="preserve">Totals</t>
+  </si>
+  <si>
     <t xml:space="preserve">Roof Structure</t>
   </si>
   <si>
+    <t xml:space="preserve">3 Universes</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADJ Vizi Beam 12RX</t>
   </si>
   <si>
@@ -151,108 +175,111 @@
     <t xml:space="preserve">ZW37s</t>
   </si>
   <si>
+    <t xml:space="preserve">Elation SixPar 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truss Warmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheeseborough 1/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Par Cans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETC S4 Series 3 Lustr X8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upstage Wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elipsoidals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work Ligts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christie B Link Bar 30° </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truss Ridgeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truss Eaves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheeseborough 90° ???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTZ Cameras ???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluminum Pipe 10' ???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety Chain 10' ???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJ Booth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Universes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jolt Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fireplace Video Wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christie B Truss 4'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christie B Truss 6'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christie B Link Bar 45° </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christie B Face Plate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheeseborough Swivel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main PA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downstage V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Universe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin Mac Viper Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage &amp; Effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vipers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downstage Wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delay Hangs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Par Can</t>
   </si>
   <si>
-    <t xml:space="preserve">Truss Warmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheeseborough 1/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Par Cans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED Color Elipsoidal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upstage Wash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elipsoidals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work Light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work Ligts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christie B Link Bar 30° </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truss Ridgeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truss Eaves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheeseborough 90° ???</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTZ Cameras ???</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluminum Pipe 10' ???</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety Chain 10' ???</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DJ Booth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jolt Bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fireplace Video Wall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christie B Truss 4'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christie B Truss 6'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christie B Link Bar 45° </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christie B Face Plate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheeseborough Swivel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main PA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rigging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Downstage V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin Mac Viper Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage &amp; Effect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vipers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED Color Ellipsoidal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Downstage Wash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delay Hangs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Room Warming</t>
   </si>
   <si>
@@ -296,9 +323,6 @@
   </si>
   <si>
     <t xml:space="preserve">Power &amp; Data Cable package TBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Totals</t>
   </si>
 </sst>
 </file>
@@ -419,12 +443,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -478,18 +502,19 @@
   </sheetPr>
   <dimension ref="A1:W129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G96" activeCellId="0" sqref="G96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16382" min="16382" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,10 +533,18 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -533,7 +566,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -549,19 +582,21 @@
       <c r="U2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="n">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -577,22 +612,27 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="n">
+        <f aca="false">F4*D4</f>
+        <v>120</v>
+      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -608,22 +648,25 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="n">
+        <f aca="false">F5*D5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -639,22 +682,25 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="n">
+        <f aca="false">F6*D6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -670,22 +716,25 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="n">
+        <f aca="false">F7*D7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -701,22 +750,27 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="n">
+        <v>127</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="n">
+        <f aca="false">F8*D8</f>
+        <v>1524</v>
+      </c>
+      <c r="I8" s="3"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -732,22 +786,25 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="n">
+        <f aca="false">F9*D9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="3"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -763,22 +820,25 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="n">
+        <f aca="false">F10*D10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -794,22 +854,25 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="n">
+        <f aca="false">F11*D11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -825,22 +888,25 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="n">
+        <f aca="false">F12*D12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -856,22 +922,25 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="n">
+        <f aca="false">F13*D13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="3"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -887,52 +956,58 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="n">
+        <f aca="false">F14*D14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="3"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="4"/>
+      <c r="O14" s="3"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
       <c r="U14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="H15" s="3" t="n">
+        <f aca="false">F15*D15</f>
+        <v>0</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -951,21 +1026,24 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="H16" s="3" t="n">
+        <f aca="false">F16*D16</f>
+        <v>0</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -984,21 +1062,24 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="4" t="n">
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="H17" s="3" t="n">
+        <f aca="false">F17*D17</f>
+        <v>0</v>
+      </c>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1017,21 +1098,26 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="4" t="n">
+      <c r="D18" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="H18" s="3" t="n">
+        <f aca="false">F18*D18</f>
+        <v>56</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1050,21 +1136,24 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="3" t="n">
+        <f aca="false">F19*D19</f>
+        <v>0</v>
+      </c>
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1083,21 +1172,24 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="4" t="n">
+      <c r="D20" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="H20" s="3" t="n">
+        <f aca="false">F20*D20</f>
+        <v>0</v>
+      </c>
       <c r="I20" s="5"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -1116,21 +1208,24 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="3" t="n">
+        <f aca="false">F21*D21</f>
+        <v>0</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -1149,21 +1244,24 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="3" t="n">
+        <f aca="false">F22*D22</f>
+        <v>0</v>
+      </c>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -1182,21 +1280,24 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="H23" s="3" t="n">
+        <f aca="false">F23*D23</f>
+        <v>0</v>
+      </c>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -1215,21 +1316,24 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="3" t="n">
+        <f aca="false">F24*D24</f>
+        <v>0</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
@@ -1251,10 +1355,15 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <f aca="false">SUM(H4:H24)</f>
+        <v>1700</v>
+      </c>
       <c r="I25" s="5"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1272,18 +1381,20 @@
       <c r="W25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>36</v>
+      <c r="A26" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="3" t="n">
         <v>6</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="H26" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I26" s="5"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -1302,21 +1413,26 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="n">
+        <v>17</v>
+      </c>
       <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="H27" s="3" t="n">
+        <f aca="false">F27*D27</f>
+        <v>306</v>
+      </c>
       <c r="I27" s="5"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -1335,21 +1451,24 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="H28" s="3" t="n">
+        <f aca="false">F28*D28</f>
+        <v>0</v>
+      </c>
       <c r="I28" s="5"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -1368,21 +1487,24 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="H29" s="3" t="n">
+        <f aca="false">F29*D29</f>
+        <v>0</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -1401,21 +1523,26 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="n">
+        <v>42</v>
+      </c>
       <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="H30" s="3" t="n">
+        <f aca="false">F30*D30</f>
+        <v>756</v>
+      </c>
       <c r="I30" s="5"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -1434,21 +1561,24 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="H31" s="3" t="n">
+        <f aca="false">F31*D31</f>
+        <v>0</v>
+      </c>
       <c r="I31" s="5"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -1467,21 +1597,24 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="H32" s="3" t="n">
+        <f aca="false">F32*D32</f>
+        <v>0</v>
+      </c>
       <c r="I32" s="5"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -1500,21 +1633,25 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="H33" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -1533,21 +1670,24 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>13</v>
+        <v>54</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D34" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="5"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
       <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="H34" s="3" t="n">
+        <f aca="false">F34*D34</f>
+        <v>0</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -1566,21 +1706,24 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>13</v>
+        <v>54</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D35" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="H35" s="3" t="n">
+        <f aca="false">F35*D35</f>
+        <v>0</v>
+      </c>
       <c r="I35" s="5"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -1599,21 +1742,26 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="3" t="n">
+        <f aca="false">F36*D36</f>
         <v>48</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -1632,21 +1780,24 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="5"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
       <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="H37" s="3" t="n">
+        <f aca="false">F37*D37</f>
+        <v>0</v>
+      </c>
       <c r="I37" s="5"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -1665,21 +1816,24 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="H38" s="3" t="n">
+        <f aca="false">F38*D38</f>
+        <v>0</v>
+      </c>
       <c r="I38" s="5"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -1697,22 +1851,27 @@
       <c r="W38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="4" t="n">
+      <c r="A39" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="5"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+      <c r="H39" s="3" t="n">
+        <f aca="false">F39*D39</f>
+        <v>16</v>
+      </c>
       <c r="I39" s="5"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -1731,21 +1890,24 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="4" t="n">
+      <c r="D40" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="5"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+      <c r="H40" s="3" t="n">
+        <f aca="false">F40*D40</f>
+        <v>0</v>
+      </c>
       <c r="I40" s="5"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -1764,21 +1926,24 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="5"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="H41" s="3" t="n">
+        <f aca="false">F41*D41</f>
+        <v>0</v>
+      </c>
       <c r="I41" s="5"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -1797,21 +1962,24 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="5"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+      <c r="H42" s="3" t="n">
+        <f aca="false">F42*D42</f>
+        <v>0</v>
+      </c>
       <c r="I42" s="5"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -1830,21 +1998,24 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="5"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="H43" s="3" t="n">
+        <f aca="false">F43*D43</f>
+        <v>0</v>
+      </c>
       <c r="I43" s="5"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
@@ -1863,21 +2034,24 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="5"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
       <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+      <c r="H44" s="3" t="n">
+        <f aca="false">F44*D44</f>
+        <v>0</v>
+      </c>
       <c r="I44" s="5"/>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
@@ -1896,21 +2070,24 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="5"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+      <c r="H45" s="3" t="n">
+        <f aca="false">F45*D45</f>
+        <v>0</v>
+      </c>
       <c r="I45" s="5"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -1929,21 +2106,24 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+      <c r="H46" s="3" t="n">
+        <f aca="false">F46*D46</f>
+        <v>0</v>
+      </c>
       <c r="I46" s="5"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
@@ -1962,21 +2142,24 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
       <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+      <c r="H47" s="3" t="n">
+        <f aca="false">F47*D47</f>
+        <v>0</v>
+      </c>
       <c r="I47" s="5"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
@@ -1995,21 +2178,24 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="4" t="n">
+        <v>65</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="5"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
       <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+      <c r="H48" s="3" t="n">
+        <f aca="false">F48*D48</f>
+        <v>0</v>
+      </c>
       <c r="I48" s="5"/>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
@@ -2028,21 +2214,24 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="4" t="n">
+        <v>66</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="5"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
       <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="H49" s="3" t="n">
+        <f aca="false">F49*D49</f>
+        <v>0</v>
+      </c>
       <c r="I49" s="5"/>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
@@ -2061,21 +2250,24 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="5"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
       <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
+      <c r="H50" s="3" t="n">
+        <f aca="false">F50*D50</f>
+        <v>0</v>
+      </c>
       <c r="I50" s="5"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
@@ -2094,21 +2286,24 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="5"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
       <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
+      <c r="H51" s="3" t="n">
+        <f aca="false">F51*D51</f>
+        <v>0</v>
+      </c>
       <c r="I51" s="5"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
@@ -2127,21 +2322,24 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="5"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
       <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
+      <c r="H52" s="3" t="n">
+        <f aca="false">F52*D52</f>
+        <v>0</v>
+      </c>
       <c r="I52" s="5"/>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
@@ -2163,10 +2361,15 @@
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <f aca="false">SUM(H27:H52)</f>
+        <v>1134</v>
+      </c>
       <c r="I53" s="5"/>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
@@ -2184,18 +2387,20 @@
       <c r="W53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
-        <v>60</v>
+      <c r="A54" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="4" t="n">
+      <c r="E54" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+      <c r="H54" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="I54" s="5"/>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
@@ -2214,53 +2419,61 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3" t="n">
+        <v>127</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3" t="n">
+        <f aca="false">F55*D55</f>
+        <v>1524</v>
+      </c>
+      <c r="I55" s="3"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
       <c r="N55" s="2"/>
-      <c r="O55" s="4"/>
+      <c r="O55" s="3"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
       <c r="U55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3" t="n">
+        <f aca="false">F56*D56</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="3"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -2276,22 +2489,25 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C57" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="4" t="n">
+      <c r="B57" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3" t="n">
+        <f aca="false">F57*D57</f>
+        <v>0</v>
+      </c>
+      <c r="I57" s="3"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
@@ -2307,22 +2523,25 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3" t="n">
+        <f aca="false">F58*D58</f>
+        <v>0</v>
+      </c>
+      <c r="I58" s="3"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
@@ -2338,22 +2557,25 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3" t="n">
+        <f aca="false">F59*D59</f>
+        <v>0</v>
+      </c>
+      <c r="I59" s="3"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -2369,22 +2591,25 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3" t="n">
+        <f aca="false">F60*D60</f>
+        <v>0</v>
+      </c>
+      <c r="I60" s="3"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -2400,21 +2625,24 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E61" s="4"/>
+      <c r="E61" s="3"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="H61" s="3" t="n">
+        <f aca="false">F61*D61</f>
+        <v>0</v>
+      </c>
       <c r="I61" s="5"/>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
@@ -2433,21 +2661,24 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="4" t="n">
+        <v>71</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="3"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
+      <c r="H62" s="3" t="n">
+        <f aca="false">F62*D62</f>
+        <v>0</v>
+      </c>
       <c r="I62" s="5"/>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
@@ -2466,21 +2697,24 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="4" t="n">
+        <v>72</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="3"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+      <c r="H63" s="3" t="n">
+        <f aca="false">F63*D63</f>
+        <v>0</v>
+      </c>
       <c r="I63" s="5"/>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
@@ -2499,21 +2733,24 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="4" t="n">
+        <v>73</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="3"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
+      <c r="H64" s="3" t="n">
+        <f aca="false">F64*D64</f>
+        <v>0</v>
+      </c>
       <c r="I64" s="5"/>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
@@ -2532,21 +2769,24 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="4" t="n">
+        <v>74</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="3"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
+      <c r="H65" s="3" t="n">
+        <f aca="false">F65*D65</f>
+        <v>0</v>
+      </c>
       <c r="I65" s="5"/>
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
@@ -2565,21 +2805,24 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E66" s="4"/>
+      <c r="E66" s="3"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
+      <c r="H66" s="3" t="n">
+        <f aca="false">F66*D66</f>
+        <v>0</v>
+      </c>
       <c r="I66" s="5"/>
       <c r="J66" s="8"/>
       <c r="K66" s="8"/>
@@ -2598,13 +2841,18 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
       <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
+      <c r="G67" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H67" s="3" t="n">
+        <f aca="false">SUM(H55:H66)</f>
+        <v>1524</v>
+      </c>
       <c r="I67" s="5"/>
       <c r="J67" s="8"/>
       <c r="K67" s="8"/>
@@ -2623,29 +2871,33 @@
     </row>
     <row r="68" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="11" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E68" s="7" t="n">
         <v>2</v>
       </c>
+      <c r="H68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E69" s="4"/>
+      <c r="E69" s="3"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
+      <c r="H69" s="3" t="n">
+        <f aca="false">F69*D69</f>
+        <v>0</v>
+      </c>
       <c r="I69" s="5"/>
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
@@ -2664,13 +2916,13 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
+      <c r="H70" s="3"/>
       <c r="I70" s="5"/>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
@@ -2688,18 +2940,20 @@
       <c r="W70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
-        <v>70</v>
+      <c r="A71" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
-      <c r="E71" s="4" t="n">
+      <c r="E71" s="3" t="n">
         <v>3</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
+      <c r="H71" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="I71" s="5"/>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
@@ -2718,21 +2972,26 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3" t="n">
+        <f aca="false">F72*D72</f>
+        <v>136</v>
+      </c>
       <c r="I72" s="5"/>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
@@ -2751,21 +3010,24 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3" t="n">
+        <f aca="false">F73*D73</f>
+        <v>0</v>
+      </c>
       <c r="I73" s="5"/>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
@@ -2784,21 +3046,24 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E74" s="4"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3" t="n">
+        <f aca="false">F74*D74</f>
+        <v>0</v>
+      </c>
       <c r="I74" s="5"/>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
@@ -2817,21 +3082,26 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="4" t="n">
+        <v>55</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="E75" s="4"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3" t="n">
+        <f aca="false">F75*D75</f>
+        <v>192</v>
+      </c>
       <c r="I75" s="5"/>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
@@ -2850,21 +3120,24 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="E76" s="4"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3" t="n">
+        <f aca="false">F76*D76</f>
+        <v>0</v>
+      </c>
       <c r="I76" s="5"/>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
@@ -2883,21 +3156,24 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D77" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
+      <c r="B77" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3" t="n">
+        <f aca="false">F77*D77</f>
+        <v>0</v>
+      </c>
       <c r="I77" s="5"/>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
@@ -2916,21 +3192,24 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3" t="n">
+        <f aca="false">F78*D78</f>
+        <v>0</v>
+      </c>
       <c r="I78" s="5"/>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
@@ -2949,21 +3228,24 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D79" s="4" t="n">
+        <v>73</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D79" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E79" s="4"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3" t="n">
+        <f aca="false">F79*D79</f>
+        <v>0</v>
+      </c>
       <c r="I79" s="5"/>
       <c r="J79" s="8"/>
       <c r="K79" s="8"/>
@@ -2982,21 +3264,24 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D80" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3" t="n">
+        <f aca="false">F80*D80</f>
+        <v>0</v>
+      </c>
       <c r="I80" s="5"/>
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
@@ -3015,21 +3300,24 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D81" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E81" s="4"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3" t="n">
+        <f aca="false">F81*D81</f>
+        <v>0</v>
+      </c>
       <c r="I81" s="5"/>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
@@ -3048,21 +3336,24 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D82" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3" t="n">
+        <f aca="false">F82*D82</f>
+        <v>0</v>
+      </c>
       <c r="I82" s="5"/>
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
@@ -3084,10 +3375,15 @@
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <f aca="false">SUM(H72:H82)</f>
+        <v>328</v>
+      </c>
       <c r="I83" s="5"/>
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
@@ -3105,18 +3401,20 @@
       <c r="W83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="s">
-        <v>76</v>
+      <c r="A84" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
-      <c r="E84" s="4" t="n">
+      <c r="E84" s="3" t="n">
         <v>3</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
+      <c r="H84" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="I84" s="5"/>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
@@ -3135,415 +3433,464 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D85" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3" t="n">
+        <f aca="false">F85*D85</f>
+        <v>96</v>
+      </c>
+      <c r="I85" s="3"/>
       <c r="J85" s="2"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
       <c r="P85" s="2"/>
-      <c r="Q85" s="4"/>
-      <c r="R85" s="4"/>
-      <c r="S85" s="4"/>
-      <c r="T85" s="4"/>
-      <c r="U85" s="4"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D86" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3" t="n">
+        <f aca="false">F86*D86</f>
+        <v>0</v>
+      </c>
+      <c r="I86" s="3"/>
       <c r="J86" s="2"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
       <c r="P86" s="2"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
-      <c r="S86" s="4"/>
-      <c r="T86" s="4"/>
-      <c r="U86" s="4"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3" t="n">
+        <f aca="false">F87*D87</f>
+        <v>0</v>
+      </c>
+      <c r="I87" s="3"/>
       <c r="J87" s="2"/>
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
       <c r="P87" s="2"/>
-      <c r="Q87" s="4"/>
-      <c r="R87" s="4"/>
-      <c r="S87" s="4"/>
-      <c r="T87" s="4"/>
-      <c r="U87" s="4"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="3"/>
+      <c r="T87" s="3"/>
+      <c r="U87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D88" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3" t="n">
+        <f aca="false">F88*D88</f>
+        <v>0</v>
+      </c>
+      <c r="I88" s="3"/>
       <c r="J88" s="2"/>
-      <c r="K88" s="4"/>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
-      <c r="N88" s="4"/>
-      <c r="O88" s="4"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
       <c r="P88" s="2"/>
-      <c r="Q88" s="4"/>
-      <c r="R88" s="4"/>
-      <c r="S88" s="4"/>
-      <c r="T88" s="4"/>
-      <c r="U88" s="4"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="3"/>
+      <c r="T88" s="3"/>
+      <c r="U88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D89" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
-      <c r="G89" s="4"/>
-      <c r="H89" s="4"/>
-      <c r="I89" s="4"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3" t="n">
+        <f aca="false">F89*D89</f>
+        <v>0</v>
+      </c>
+      <c r="I89" s="3"/>
       <c r="J89" s="2"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
-      <c r="N89" s="4"/>
-      <c r="O89" s="4"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
       <c r="P89" s="2"/>
       <c r="R89" s="2"/>
       <c r="S89" s="2"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3" t="n">
+        <f aca="false">F90*D90</f>
+        <v>0</v>
+      </c>
+      <c r="I90" s="3"/>
       <c r="J90" s="2"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
-      <c r="N90" s="4"/>
-      <c r="O90" s="4"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
       <c r="P90" s="2"/>
       <c r="R90" s="2"/>
       <c r="S90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D91" s="4" t="n">
+        <v>88</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3" t="n">
+        <f aca="false">F91*D91</f>
+        <v>0</v>
+      </c>
+      <c r="I91" s="3"/>
       <c r="J91" s="2"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
-      <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
       <c r="P91" s="2"/>
       <c r="R91" s="2"/>
       <c r="S91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D92" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D92" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3" t="n">
+        <f aca="false">F92*D92</f>
+        <v>0</v>
+      </c>
+      <c r="I92" s="3"/>
       <c r="J92" s="2"/>
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
       <c r="P92" s="2"/>
       <c r="R92" s="2"/>
       <c r="S92" s="2"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D93" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3" t="n">
+        <f aca="false">F93*D93</f>
+        <v>0</v>
+      </c>
+      <c r="I93" s="3"/>
       <c r="J93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
-      <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="3"/>
       <c r="P93" s="2"/>
       <c r="R93" s="2"/>
       <c r="S93" s="2"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D94" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
-      <c r="I94" s="4"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3" t="n">
+        <f aca="false">F94*D94</f>
+        <v>0</v>
+      </c>
+      <c r="I94" s="3"/>
       <c r="J94" s="2"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
-      <c r="N94" s="4"/>
-      <c r="O94" s="4"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="3"/>
       <c r="P94" s="2"/>
       <c r="R94" s="2"/>
       <c r="S94" s="2"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H95" s="3" t="n">
+        <f aca="false">SUM(H85:H94)</f>
+        <v>96</v>
+      </c>
+      <c r="I95" s="3"/>
       <c r="J95" s="2"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
-      <c r="N95" s="4"/>
-      <c r="O95" s="4"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
       <c r="P95" s="2"/>
       <c r="R95" s="2"/>
       <c r="S95" s="2"/>
     </row>
     <row r="96" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F96" s="4"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
+      <c r="A96" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
       <c r="J96" s="2"/>
-      <c r="K96" s="4"/>
+      <c r="K96" s="3"/>
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
-      <c r="N96" s="4"/>
-      <c r="O96" s="4"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="3"/>
       <c r="P96" s="2"/>
-      <c r="Q96" s="4"/>
+      <c r="Q96" s="3"/>
       <c r="R96" s="2"/>
       <c r="S96" s="2"/>
-      <c r="T96" s="4"/>
-      <c r="U96" s="4"/>
+      <c r="T96" s="3"/>
+      <c r="U96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D97" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D97" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3" t="n">
+        <f aca="false">F97*D97</f>
+        <v>0</v>
+      </c>
+      <c r="I97" s="3"/>
       <c r="J97" s="2"/>
-      <c r="K97" s="4"/>
-      <c r="L97" s="4"/>
-      <c r="M97" s="4"/>
-      <c r="N97" s="4"/>
-      <c r="O97" s="4"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="3"/>
       <c r="P97" s="2"/>
-      <c r="Q97" s="4"/>
-      <c r="R97" s="4"/>
-      <c r="S97" s="4"/>
-      <c r="T97" s="4"/>
-      <c r="U97" s="4"/>
+      <c r="Q97" s="3"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="3"/>
+      <c r="T97" s="3"/>
+      <c r="U97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D98" s="4" t="n">
+        <v>91</v>
+      </c>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
-      <c r="I98" s="4"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3" t="n">
+        <f aca="false">F98*D98</f>
+        <v>0</v>
+      </c>
+      <c r="I98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D99" s="4" t="n">
+        <v>92</v>
+      </c>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D99" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3" t="n">
+        <f aca="false">F99*D99</f>
+        <v>0</v>
+      </c>
+      <c r="I99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D100" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3" t="n">
+        <f aca="false">F100*D100</f>
+        <v>0</v>
+      </c>
+      <c r="I100" s="3"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
@@ -3559,20 +3906,23 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D101" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3" t="n">
+        <f aca="false">F101*D101</f>
+        <v>0</v>
+      </c>
+      <c r="I101" s="3"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
@@ -3588,99 +3938,105 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D102" s="4" t="n">
+        <v>94</v>
+      </c>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D102" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E102" s="4"/>
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
-      <c r="I102" s="4"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3" t="n">
+        <f aca="false">F102*D102</f>
+        <v>0</v>
+      </c>
+      <c r="I102" s="3"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
-      <c r="L102" s="4"/>
+      <c r="L102" s="3"/>
       <c r="M102" s="2"/>
-      <c r="N102" s="4"/>
+      <c r="N102" s="3"/>
       <c r="O102" s="2"/>
-      <c r="P102" s="4"/>
+      <c r="P102" s="3"/>
       <c r="Q102" s="2"/>
       <c r="R102" s="2"/>
-      <c r="S102" s="4"/>
+      <c r="S102" s="3"/>
       <c r="T102" s="2"/>
-      <c r="U102" s="4"/>
+      <c r="U102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
-      <c r="L103" s="4"/>
+      <c r="L103" s="3"/>
       <c r="M103" s="2"/>
-      <c r="N103" s="4"/>
+      <c r="N103" s="3"/>
       <c r="O103" s="2"/>
-      <c r="P103" s="4"/>
+      <c r="P103" s="3"/>
       <c r="Q103" s="2"/>
       <c r="R103" s="2"/>
-      <c r="S103" s="4"/>
+      <c r="S103" s="3"/>
       <c r="T103" s="2"/>
-      <c r="U103" s="4"/>
+      <c r="U103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
+      <c r="A104" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
-      <c r="L104" s="4"/>
+      <c r="L104" s="3"/>
       <c r="M104" s="2"/>
-      <c r="N104" s="4"/>
+      <c r="N104" s="3"/>
       <c r="O104" s="2"/>
-      <c r="P104" s="4"/>
+      <c r="P104" s="3"/>
       <c r="Q104" s="2"/>
       <c r="R104" s="2"/>
-      <c r="S104" s="4"/>
+      <c r="S104" s="3"/>
       <c r="T104" s="2"/>
-      <c r="U104" s="4"/>
+      <c r="U104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D105" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3" t="n">
+        <f aca="false">F105*D105</f>
+        <v>0</v>
+      </c>
+      <c r="I105" s="3"/>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
@@ -3696,20 +4052,23 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D106" s="4" t="n">
+        <v>97</v>
+      </c>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3" t="n">
+        <f aca="false">F106*D106</f>
+        <v>0</v>
+      </c>
+      <c r="I106" s="3"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
@@ -3725,20 +4084,23 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D107" s="4" t="n">
+        <v>98</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D107" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
-      <c r="I107" s="4"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3" t="n">
+        <f aca="false">F107*D107</f>
+        <v>0</v>
+      </c>
+      <c r="I107" s="3"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
@@ -3754,20 +4116,23 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D108" s="4" t="n">
+        <v>99</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D108" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
-      <c r="I108" s="4"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3" t="n">
+        <f aca="false">F108*D108</f>
+        <v>0</v>
+      </c>
+      <c r="I108" s="3"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
@@ -3783,20 +4148,23 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D109" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D109" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
-      <c r="I109" s="4"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3" t="n">
+        <f aca="false">F109*D109</f>
+        <v>0</v>
+      </c>
+      <c r="I109" s="3"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
@@ -3812,14 +4180,14 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
@@ -3835,16 +4203,16 @@
     </row>
     <row r="111" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
-      <c r="I111" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
@@ -3860,17 +4228,17 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4" t="n">
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3" t="n">
         <f aca="false">SUM(E2:E105)</f>
         <v>16</v>
       </c>
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
@@ -3886,14 +4254,14 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
@@ -3909,14 +4277,14 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
-      <c r="G114" s="4"/>
-      <c r="H114" s="4"/>
-      <c r="I114" s="4"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
+      <c r="I114" s="3"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
@@ -3932,20 +4300,20 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2"/>
-      <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4"/>
-      <c r="E115" s="4"/>
-      <c r="F115" s="4"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
-      <c r="I115" s="4"/>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
-      <c r="N115" s="4"/>
-      <c r="O115" s="4"/>
+      <c r="N115" s="3"/>
+      <c r="O115" s="3"/>
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
       <c r="R115" s="2"/>
@@ -3955,14 +4323,14 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
-      <c r="G116" s="4"/>
-      <c r="H116" s="4"/>
-      <c r="I116" s="4"/>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+      <c r="I116" s="3"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
@@ -3978,14 +4346,14 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
-      <c r="G117" s="4"/>
-      <c r="H117" s="4"/>
-      <c r="I117" s="4"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+      <c r="I117" s="3"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
@@ -4001,21 +4369,21 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="4"/>
-      <c r="G118" s="4"/>
-      <c r="H118" s="4"/>
-      <c r="I118" s="4"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
-      <c r="L118" s="4"/>
-      <c r="M118" s="4"/>
-      <c r="N118" s="4"/>
-      <c r="O118" s="4"/>
-      <c r="P118" s="4"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="3"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="3"/>
+      <c r="P118" s="3"/>
       <c r="Q118" s="2"/>
       <c r="R118" s="2"/>
       <c r="S118" s="2"/>
@@ -4024,14 +4392,14 @@
     </row>
     <row r="119" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="2"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
-      <c r="G119" s="4"/>
-      <c r="H119" s="4"/>
-      <c r="I119" s="4"/>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3"/>
+      <c r="I119" s="3"/>
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
@@ -4046,14 +4414,14 @@
       <c r="U119" s="2"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="3"/>
+      <c r="I120" s="3"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
@@ -4067,14 +4435,14 @@
       <c r="T120" s="2"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
-      <c r="I121" s="4"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
@@ -4088,14 +4456,14 @@
       <c r="T121" s="2"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="4"/>
-      <c r="H122" s="4"/>
-      <c r="I122" s="4"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
@@ -4109,67 +4477,67 @@
       <c r="T122" s="2"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4"/>
-      <c r="H124" s="4"/>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4"/>
-      <c r="E125" s="4"/>
-      <c r="F125" s="4"/>
-      <c r="G125" s="4"/>
-      <c r="H125" s="4"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
+      <c r="H125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4"/>
-      <c r="E126" s="4"/>
-      <c r="F126" s="4"/>
-      <c r="G126" s="4"/>
-      <c r="H126" s="4"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="4"/>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4"/>
-      <c r="E127" s="4"/>
-      <c r="F127" s="4"/>
-      <c r="G127" s="4"/>
-      <c r="H127" s="4"/>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="4"/>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4"/>
-      <c r="E128" s="4"/>
-      <c r="F128" s="4"/>
-      <c r="G128" s="4"/>
-      <c r="H128" s="4"/>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
+      <c r="H128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="4"/>
-      <c r="C129" s="4"/>
-      <c r="D129" s="4"/>
-      <c r="E129" s="4"/>
-      <c r="F129" s="4"/>
-      <c r="G129" s="4"/>
-      <c r="H129" s="4"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Finalize cables and patch
</commit_message>
<xml_diff>
--- a/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.10.xlsx
+++ b/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.10.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Gear List" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Gear List" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="DMX" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Power" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="119">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -338,6 +340,45 @@
   </si>
   <si>
     <t xml:space="preserve">Power &amp; Data Cable package TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XLR-5 Cable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socapex 19 Pin 12/14 Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE1 14/3 Break-Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edison 5-15 12/3 Break-Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE1 14/3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edison 5-15 12/3 Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twofer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Bar</t>
   </si>
 </sst>
 </file>
@@ -445,7 +486,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -506,6 +547,18 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,6 +571,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -525,10 +684,10 @@
   </sheetPr>
   <dimension ref="A1:X130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="H65" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="H2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L76" activeCellId="0" sqref="L76"/>
+      <selection pane="bottomLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5096,4 +5255,1213 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.51"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <f aca="false">C4*B4</f>
+        <v>120</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="G4" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>127</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <f aca="false">C5*B5</f>
+        <v>1524</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="G5" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <f aca="false">C6*B6</f>
+        <v>56</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="G6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3" t="n">
+        <f aca="false">SUM(D4:D6)</f>
+        <v>1700</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <f aca="false">C9*B9</f>
+        <v>306</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="G9" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <f aca="false">C10*B10</f>
+        <v>756</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="G10" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="G11" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <f aca="false">C12*B12</f>
+        <v>48</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="H12" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <f aca="false">C13*B13</f>
+        <v>16</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="H13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="n">
+        <f aca="false">SUM(D9:D13)</f>
+        <v>1134</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>127</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <f aca="false">C16*B16</f>
+        <v>1524</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="G16" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <f aca="false">C17*B17</f>
+        <v>6</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="I17" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3" t="n">
+        <f aca="false">SUM(D16:D16)</f>
+        <v>1524</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <f aca="false">C20*B20</f>
+        <v>136</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="G20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <f aca="false">C21*B21</f>
+        <v>192</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="G21" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="n">
+        <f aca="false">SUM(D20:D21)</f>
+        <v>328</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <f aca="false">C24*B24</f>
+        <v>96</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="G24" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="n">
+        <f aca="false">SUM(D24:D24)</f>
+        <v>96</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="n">
+        <f aca="false">SUM(E3:E25)</f>
+        <v>15</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">SUM(G3:G25)</f>
+        <v>107</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">SUM(H3:H25)</f>
+        <v>7</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">SUM(I3:I25)</f>
+        <v>6</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">SUM(J3:J25)</f>
+        <v>15</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">SUM(K3:K25)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:W27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.02"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <f aca="false">B4*C4</f>
+        <v>10.8</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <f aca="false">B5*C5</f>
+        <v>39.6</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <f aca="false">B6*C6</f>
+        <v>3.29</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <f aca="false">SUM(D4:D6)</f>
+        <v>53.69</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <f aca="false">B9*C9</f>
+        <v>32.4</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <f aca="false">B10*C10</f>
+        <v>61.2</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <f aca="false">B11*C11</f>
+        <v>12.6</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <f aca="false">B12*C12</f>
+        <v>7.2</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <f aca="false">B13*C13</f>
+        <v>0.54</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <f aca="false">SUM(D9:D13)</f>
+        <v>113.94</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <f aca="false">B16*C16</f>
+        <v>39.6</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="13" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <f aca="false">B17*C17</f>
+        <v>21.6</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <f aca="false">SUM(D16:D16)</f>
+        <v>39.6</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <f aca="false">B20*C20</f>
+        <v>23.2</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <f aca="false">B21*C21</f>
+        <v>28.8</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <f aca="false">SUM(D20:D21)</f>
+        <v>52</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <f aca="false">B24*C24</f>
+        <v>8.4</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <f aca="false">SUM(D24:D24)</f>
+        <v>8.4</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="H27" s="0" t="n">
+        <f aca="false">SUM(H3:H25)</f>
+        <v>4</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">SUM(I3:I25)</f>
+        <v>3</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">SUM(J3:J25)</f>
+        <v>3</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">SUM(K3:K25)</f>
+        <v>3</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <f aca="false">SUM(L3:L25)</f>
+        <v>64</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <f aca="false">SUM(M3:M25)</f>
+        <v>30</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <f aca="false">SUM(N3:N25)</f>
+        <v>6</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <f aca="false">SUM(O3:O25)</f>
+        <v>2</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <f aca="false">SUM(P3:P25)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <f aca="false">SUM(Q3:Q25)</f>
+        <v>25</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <f aca="false">SUM(R3:R25)</f>
+        <v>4</v>
+      </c>
+      <c r="S27" s="0" t="n">
+        <f aca="false">SUM(S3:S25)</f>
+        <v>1</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <f aca="false">SUM(T3:T25)</f>
+        <v>2</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <f aca="false">SUM(U3:U25)</f>
+        <v>0</v>
+      </c>
+      <c r="V27" s="0" t="n">
+        <f aca="false">SUM(V3:V25)</f>
+        <v>7</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <f aca="false">SUM(W3:W25)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:W1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>